<commit_message>
a more further effect o the statistical testing
</commit_message>
<xml_diff>
--- a/Hypertension/Summary tables.xlsx
+++ b/Hypertension/Summary tables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>Variable</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Has Hypertension/Salt Intake</t>
   </si>
 </sst>
 </file>
@@ -147,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -174,6 +180,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -456,15 +468,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:K16"/>
+  <dimension ref="C3:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="2" customWidth="1"/>
     <col min="4" max="11" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -751,6 +763,202 @@
         <v>32</v>
       </c>
     </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="3:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="C20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="10">
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="E21" s="10">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="F21" s="10">
+        <v>1.88</v>
+      </c>
+      <c r="G21" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="H21" s="10">
+        <v>7.1</v>
+      </c>
+      <c r="I21" s="10">
+        <v>9.5</v>
+      </c>
+      <c r="J21" s="10">
+        <v>14.8</v>
+      </c>
+      <c r="K21" s="10">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="11">
+        <v>8.75</v>
+      </c>
+      <c r="E22" s="11">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F22" s="11">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="G22" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="H22" s="11">
+        <v>7.3</v>
+      </c>
+      <c r="I22" s="11">
+        <v>10.3</v>
+      </c>
+      <c r="J22" s="11">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="K22" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="1">
+        <v>4.37</v>
+      </c>
+      <c r="E26" s="1">
+        <v>4</v>
+      </c>
+      <c r="F26" s="1">
+        <v>2.87</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>2</v>
+      </c>
+      <c r="I26" s="1">
+        <v>6</v>
+      </c>
+      <c r="J26" s="1">
+        <v>10</v>
+      </c>
+      <c r="K26" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C27" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="9">
+        <v>5.54</v>
+      </c>
+      <c r="E27" s="9">
+        <v>6</v>
+      </c>
+      <c r="F27" s="9">
+        <v>3.28</v>
+      </c>
+      <c r="G27" s="9">
+        <v>0</v>
+      </c>
+      <c r="H27" s="9">
+        <v>3</v>
+      </c>
+      <c r="I27" s="9">
+        <v>9</v>
+      </c>
+      <c r="J27" s="9">
+        <v>10</v>
+      </c>
+      <c r="K27" s="9">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
moving forward with the analysis
</commit_message>
<xml_diff>
--- a/Hypertension/Summary tables.xlsx
+++ b/Hypertension/Summary tables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="34">
   <si>
     <t>Variable</t>
   </si>
@@ -90,6 +90,42 @@
   </si>
   <si>
     <t>Has Hypertension/Salt Intake</t>
+  </si>
+  <si>
+    <t>Has Hypertension/Sleep Duration</t>
+  </si>
+  <si>
+    <t>Has Hypertension/BMI</t>
+  </si>
+  <si>
+    <t>Hypertension (%)</t>
+  </si>
+  <si>
+    <t>Normal (%)</t>
+  </si>
+  <si>
+    <t>Prehypertension (%)</t>
+  </si>
+  <si>
+    <t>ACE Inhibitor (%)</t>
+  </si>
+  <si>
+    <t>Beta Blocker (%)</t>
+  </si>
+  <si>
+    <t>Diuretic (%)</t>
+  </si>
+  <si>
+    <t>None (%)</t>
+  </si>
+  <si>
+    <t>Other (%)</t>
+  </si>
+  <si>
+    <t>No (%)</t>
+  </si>
+  <si>
+    <t>Yes (%)</t>
   </si>
 </sst>
 </file>
@@ -153,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -182,11 +218,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -468,19 +529,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:K27"/>
+  <dimension ref="C3:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="22.85546875" style="2" customWidth="1"/>
     <col min="4" max="11" width="9.140625" style="2"/>
+    <col min="14" max="14" width="15.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -490,8 +555,12 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+    </row>
+    <row r="4" spans="3:19" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
@@ -519,8 +588,20 @@
       <c r="K4" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
@@ -548,8 +629,20 @@
       <c r="K5" s="1">
         <v>84</v>
       </c>
-    </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N5" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="13">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="P5" s="13">
+        <v>0.53520000000000001</v>
+      </c>
+      <c r="Q5" s="13">
+        <v>0.42180000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C6" s="3" t="s">
         <v>7</v>
       </c>
@@ -577,8 +670,20 @@
       <c r="K6" s="1">
         <v>16.399999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N6" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" s="14">
+        <v>0.51160000000000005</v>
+      </c>
+      <c r="P6" s="14">
+        <v>0.27710000000000001</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>0.2112</v>
+      </c>
+    </row>
+    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
         <v>8</v>
       </c>
@@ -607,7 +712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
@@ -636,7 +741,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="s">
         <v>10</v>
       </c>
@@ -664,8 +769,74 @@
       <c r="K9" s="9">
         <v>41.9</v>
       </c>
-    </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+    </row>
+    <row r="10" spans="3:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="N10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="N11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O11" s="17">
+        <v>0.17</v>
+      </c>
+      <c r="P11" s="17">
+        <v>0.20780000000000001</v>
+      </c>
+      <c r="Q11" s="17">
+        <v>0.11119999999999999</v>
+      </c>
+      <c r="R11" s="17">
+        <v>0.40610000000000002</v>
+      </c>
+      <c r="S11" s="17">
+        <v>0.10489999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="N12" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="O12" s="19">
+        <v>0.156</v>
+      </c>
+      <c r="P12" s="19">
+        <v>0.2074</v>
+      </c>
+      <c r="Q12" s="19">
+        <v>0.13469999999999999</v>
+      </c>
+      <c r="R12" s="19">
+        <v>0.3992</v>
+      </c>
+      <c r="S12" s="19">
+        <v>0.1027</v>
+      </c>
+    </row>
+    <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -676,7 +847,7 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="3:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:19" ht="30" x14ac:dyDescent="0.25">
       <c r="C14" s="6" t="s">
         <v>11</v>
       </c>
@@ -704,8 +875,11 @@
       <c r="K14" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+    </row>
+    <row r="15" spans="3:19" ht="30" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
         <v>18</v>
       </c>
@@ -733,8 +907,17 @@
       <c r="K15" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C16" s="9" t="s">
         <v>19</v>
       </c>
@@ -762,8 +945,28 @@
       <c r="K16" s="9">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O16" s="17">
+        <v>0.65059999999999996</v>
+      </c>
+      <c r="P16" s="17">
+        <v>0.34939999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="O17" s="19">
+        <v>0.36820000000000003</v>
+      </c>
+      <c r="P17" s="19">
+        <v>0.63180000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -774,7 +977,7 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="3:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" ht="30" x14ac:dyDescent="0.25">
       <c r="C20" s="6" t="s">
         <v>21</v>
       </c>
@@ -803,65 +1006,65 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C21" s="10" t="s">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C21" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="11">
         <v>8.2899999999999991</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="11">
         <v>8.3000000000000007</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="11">
         <v>1.88</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="11">
         <v>2.5</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H21" s="11">
         <v>7.1</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="11">
         <v>9.5</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="11">
         <v>14.8</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K21" s="11">
         <v>2.4</v>
       </c>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="11" t="s">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="12">
         <v>8.75</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="12">
         <v>8.6999999999999993</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="12">
         <v>2.0699999999999998</v>
       </c>
-      <c r="G22" s="11">
+      <c r="G22" s="12">
         <v>2.5</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H22" s="12">
         <v>7.3</v>
       </c>
-      <c r="I22" s="11">
+      <c r="I22" s="12">
         <v>10.3</v>
       </c>
-      <c r="J22" s="11">
+      <c r="J22" s="12">
         <v>16.399999999999999</v>
       </c>
-      <c r="K22" s="11">
+      <c r="K22" s="12">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -872,7 +1075,7 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
     </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C25" s="6" t="s">
         <v>11</v>
       </c>
@@ -901,7 +1104,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>18</v>
       </c>
@@ -930,7 +1133,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C27" s="9" t="s">
         <v>19</v>
       </c>
@@ -957,6 +1160,202 @@
       </c>
       <c r="K27" s="9">
         <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="3:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="C30" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="1">
+        <v>6.64</v>
+      </c>
+      <c r="E31" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1.38</v>
+      </c>
+      <c r="G31" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H31" s="1">
+        <v>5.7</v>
+      </c>
+      <c r="I31" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="J31" s="1">
+        <v>11</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C32" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="9">
+        <v>6.28</v>
+      </c>
+      <c r="E32" s="9">
+        <v>6.3</v>
+      </c>
+      <c r="F32" s="9">
+        <v>1.66</v>
+      </c>
+      <c r="G32" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="H32" s="9">
+        <v>5</v>
+      </c>
+      <c r="I32" s="9">
+        <v>7.4</v>
+      </c>
+      <c r="J32" s="9">
+        <v>11.4</v>
+      </c>
+      <c r="K32" s="9">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C35" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="1">
+        <v>25.33</v>
+      </c>
+      <c r="E36" s="1">
+        <v>25.4</v>
+      </c>
+      <c r="F36" s="1">
+        <v>4.18</v>
+      </c>
+      <c r="G36" s="1">
+        <v>11.9</v>
+      </c>
+      <c r="H36" s="1">
+        <v>22.7</v>
+      </c>
+      <c r="I36" s="1">
+        <v>28.2</v>
+      </c>
+      <c r="J36" s="1">
+        <v>38.4</v>
+      </c>
+      <c r="K36" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C37" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="9">
+        <v>26.64</v>
+      </c>
+      <c r="E37" s="9">
+        <v>26.6</v>
+      </c>
+      <c r="F37" s="9">
+        <v>4.71</v>
+      </c>
+      <c r="G37" s="9">
+        <v>13.4</v>
+      </c>
+      <c r="H37" s="9">
+        <v>23.4</v>
+      </c>
+      <c r="I37" s="9">
+        <v>30.2</v>
+      </c>
+      <c r="J37" s="9">
+        <v>41.9</v>
+      </c>
+      <c r="K37" s="9">
+        <v>6.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edditing my word document
</commit_message>
<xml_diff>
--- a/Hypertension/Summary tables.xlsx
+++ b/Hypertension/Summary tables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="51">
   <si>
     <t>Variable</t>
   </si>
@@ -150,6 +150,33 @@
   </si>
   <si>
     <t>Smoker</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1-score</t>
+  </si>
+  <si>
+    <t>Support</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>Macro Avg</t>
+  </si>
+  <si>
+    <t>Weighted Avg</t>
   </si>
 </sst>
 </file>
@@ -213,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -277,6 +304,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -559,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:S37"/>
+  <dimension ref="C3:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="G24" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,7 +1402,7 @@
         <v>0.71830000000000005</v>
       </c>
     </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -1383,7 +1413,7 @@
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C35" s="6" t="s">
         <v>23</v>
       </c>
@@ -1411,8 +1441,13 @@
       <c r="K35" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="18"/>
+    </row>
+    <row r="36" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C36" s="1" t="s">
         <v>18</v>
       </c>
@@ -1440,8 +1475,23 @@
       <c r="K36" s="1">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N36" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="O36" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="P36" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q36" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="R36" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="3:18" x14ac:dyDescent="0.25">
       <c r="C37" s="9" t="s">
         <v>19</v>
       </c>
@@ -1468,6 +1518,198 @@
       </c>
       <c r="K37" s="9">
         <v>6.8</v>
+      </c>
+      <c r="N37" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O37" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="P37" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="R37" s="1">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="38" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="N38" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="O38" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="P38" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="R38" s="1">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="39" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="N39" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q39" s="23">
+        <v>0.85</v>
+      </c>
+      <c r="R39" s="23">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="40" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="N40" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="O40" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="P40" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="R40" s="1">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="41" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="N41" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="O41" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="P41" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="Q41" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="R41" s="9">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="43" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="18"/>
+    </row>
+    <row r="44" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="N44" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="O44" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="P44" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q44" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="R44" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="N45" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O45" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="P45" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="R45" s="1">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="46" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="N46" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O46" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="P46" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="R46" s="1">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="47" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="N47" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O47" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P47" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q47" s="23">
+        <v>0.84</v>
+      </c>
+      <c r="R47" s="23">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="48" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="N48" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="O48" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="P48" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="R48" s="1">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="49" spans="14:18" x14ac:dyDescent="0.25">
+      <c r="N49" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="O49" s="9">
+        <v>0.84</v>
+      </c>
+      <c r="P49" s="9">
+        <v>0.84</v>
+      </c>
+      <c r="Q49" s="9">
+        <v>0.84</v>
+      </c>
+      <c r="R49" s="9">
+        <v>397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>